<commit_message>
ADAM DAK Sprint #1
</commit_message>
<xml_diff>
--- a/config/forms/contact/health_unit-edit.xlsx
+++ b/config/forms/contact/health_unit-edit.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\morlig\icap\dmi-adam-zwei\config\forms\contact\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\morlig\icap\dmi-adam-repositories\dmi-adam\config\forms\contact\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F41A2A0-CA75-40A7-B8E1-AB5AA8E9868C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0678E77-F274-43FF-BD6E-981456CA4CE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="57">
   <si>
     <t>type</t>
   </si>
@@ -46,24 +46,9 @@
     <t>label::en</t>
   </si>
   <si>
-    <t>label::hi</t>
-  </si>
-  <si>
-    <t>label::id</t>
-  </si>
-  <si>
     <t>label::sw</t>
   </si>
   <si>
-    <t>label::ne</t>
-  </si>
-  <si>
-    <t>label::es</t>
-  </si>
-  <si>
-    <t>label::fr</t>
-  </si>
-  <si>
     <t>required</t>
   </si>
   <si>
@@ -91,9 +76,6 @@
     <t>hint::en</t>
   </si>
   <si>
-    <t>hint::sw</t>
-  </si>
-  <si>
     <t>default</t>
   </si>
   <si>
@@ -154,24 +136,6 @@
     <t>PARENT</t>
   </si>
   <si>
-    <t>external_id</t>
-  </si>
-  <si>
-    <t>External ID</t>
-  </si>
-  <si>
-    <t>बाहरी ID</t>
-  </si>
-  <si>
-    <t>Eksternal ID</t>
-  </si>
-  <si>
-    <t>बाहिरि ID</t>
-  </si>
-  <si>
-    <t>Identifiant externe</t>
-  </si>
-  <si>
     <t>meta</t>
   </si>
   <si>
@@ -196,21 +160,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>नाम</t>
-  </si>
-  <si>
-    <t>Nama</t>
-  </si>
-  <si>
-    <t>Jina</t>
-  </si>
-  <si>
-    <t>Nom</t>
-  </si>
-  <si>
-    <t>Namba ya nje</t>
-  </si>
-  <si>
     <t>list_name</t>
   </si>
   <si>
@@ -250,13 +199,7 @@
     <t>en</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>no</t>
-  </si>
-  <si>
-    <t>description</t>
   </si>
   <si>
     <t>contact:PLACE_TYPE:edit</t>
@@ -269,11 +212,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="64"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -287,24 +237,12 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFF2CC"/>
-        <bgColor rgb="FFFFF2CC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFCE5CD"/>
-        <bgColor rgb="FFFCE5CD"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -314,38 +252,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD0E0E3"/>
-        <bgColor rgb="FFD0E0E3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD9D2E9"/>
-        <bgColor rgb="FFD9D2E9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCFE2F3"/>
-        <bgColor rgb="FFCFE2F3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD9D9D9"/>
-        <bgColor rgb="FFD9D9D9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF3F3F3"/>
-        <bgColor rgb="FFF3F3F3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF6FA8DC"/>
-        <bgColor rgb="FF6FA8DC"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -358,50 +266,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="60% - Accent1" xfId="1" builtinId="32"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -627,44 +511,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM949"/>
+  <dimension ref="A1:N948"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C2" sqref="C2"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="47.81640625" customWidth="1"/>
-    <col min="4" max="4" width="33.453125" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="27.453125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="37.26953125" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="31.26953125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="8.08984375" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="16.7265625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="8.08984375" customWidth="1"/>
-    <col min="11" max="11" width="51.453125" customWidth="1"/>
-    <col min="12" max="13" width="10.7265625" customWidth="1"/>
-    <col min="14" max="14" width="25.26953125" customWidth="1"/>
-    <col min="15" max="15" width="46.26953125" customWidth="1"/>
-    <col min="16" max="16" width="68.81640625" customWidth="1"/>
-    <col min="17" max="17" width="9.453125" customWidth="1"/>
-    <col min="18" max="18" width="33.453125" customWidth="1"/>
-    <col min="19" max="19" width="13.54296875" customWidth="1"/>
-    <col min="20" max="20" width="8.7265625" customWidth="1"/>
-    <col min="21" max="21" width="35.81640625" customWidth="1"/>
-    <col min="22" max="31" width="7.7265625" customWidth="1"/>
-    <col min="32" max="33" width="15.08984375" customWidth="1"/>
-    <col min="34" max="39" width="17.26953125" customWidth="1"/>
+    <col min="3" max="3" width="39.54296875" customWidth="1"/>
+    <col min="4" max="4" width="8.08984375" customWidth="1"/>
+    <col min="5" max="5" width="51.453125" customWidth="1"/>
+    <col min="6" max="7" width="10.7265625" customWidth="1"/>
+    <col min="8" max="8" width="25.26953125" customWidth="1"/>
+    <col min="9" max="9" width="46.26953125" customWidth="1"/>
+    <col min="10" max="10" width="68.81640625" customWidth="1"/>
+    <col min="11" max="11" width="9.453125" customWidth="1"/>
+    <col min="12" max="12" width="33.453125" customWidth="1"/>
+    <col min="13" max="13" width="8.7265625" customWidth="1"/>
+    <col min="14" max="14" width="35.81640625" customWidth="1"/>
+    <col min="15" max="24" width="7.7265625" customWidth="1"/>
+    <col min="25" max="26" width="15.08984375" customWidth="1"/>
+    <col min="27" max="32" width="17.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -674,1095 +551,242 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:14" s="7" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="B2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="C2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9" t="b">
+      <c r="E2" s="7" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9"/>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9"/>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="9"/>
-      <c r="AC2" s="9"/>
-      <c r="AD2" s="9"/>
-      <c r="AE2" s="9"/>
-      <c r="AF2" s="9"/>
-      <c r="AG2" s="9"/>
-      <c r="AH2" s="9"/>
-      <c r="AI2" s="9"/>
-      <c r="AJ2" s="9"/>
-      <c r="AK2" s="9"/>
-      <c r="AL2" s="9"/>
-      <c r="AM2" s="9"/>
     </row>
-    <row r="3" spans="1:39" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:14" s="7" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="8" t="s">
+    </row>
+    <row r="5" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="N6" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="9"/>
-      <c r="V3" s="9"/>
-      <c r="W3" s="9"/>
-      <c r="X3" s="9"/>
-      <c r="Y3" s="9"/>
-      <c r="Z3" s="9"/>
-      <c r="AA3" s="9"/>
-      <c r="AB3" s="9"/>
-      <c r="AC3" s="9"/>
-      <c r="AD3" s="9"/>
-      <c r="AE3" s="9"/>
-      <c r="AF3" s="9"/>
-      <c r="AG3" s="9"/>
-      <c r="AH3" s="9"/>
-      <c r="AI3" s="9"/>
-      <c r="AJ3" s="9"/>
-      <c r="AK3" s="9"/>
-      <c r="AL3" s="9"/>
-      <c r="AM3" s="9"/>
     </row>
-    <row r="4" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
+    <row r="7" spans="1:14" s="7" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="8" t="s">
+    </row>
+    <row r="8" spans="1:14" s="7" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:14" s="7" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9" t="s">
+    </row>
+    <row r="11" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="M11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
         <v>27</v>
       </c>
-      <c r="V4" s="9"/>
-      <c r="W4" s="9"/>
-      <c r="X4" s="9"/>
-      <c r="Y4" s="9"/>
-      <c r="Z4" s="9"/>
-      <c r="AA4" s="9"/>
-      <c r="AB4" s="9"/>
-      <c r="AC4" s="9"/>
-      <c r="AD4" s="9"/>
-      <c r="AE4" s="9"/>
-      <c r="AF4" s="9"/>
-      <c r="AG4" s="9"/>
-      <c r="AH4" s="9"/>
-      <c r="AI4" s="9"/>
-      <c r="AJ4" s="9"/>
-      <c r="AK4" s="9"/>
-      <c r="AL4" s="9"/>
-      <c r="AM4" s="9"/>
     </row>
-    <row r="5" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="8" t="s">
+    <row r="14" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:14" s="7" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="J16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="J17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="J18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="7" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9"/>
-      <c r="S5" s="9"/>
-      <c r="T5" s="9"/>
-      <c r="U5" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="V5" s="9"/>
-      <c r="W5" s="9"/>
-      <c r="X5" s="9"/>
-      <c r="Y5" s="9"/>
-      <c r="Z5" s="9"/>
-      <c r="AA5" s="9"/>
-      <c r="AB5" s="9"/>
-      <c r="AC5" s="9"/>
-      <c r="AD5" s="9"/>
-      <c r="AE5" s="9"/>
-      <c r="AF5" s="9"/>
-      <c r="AG5" s="9"/>
-      <c r="AH5" s="9"/>
-      <c r="AI5" s="9"/>
-      <c r="AJ5" s="9"/>
-      <c r="AK5" s="9"/>
-      <c r="AL5" s="9"/>
-      <c r="AM5" s="9"/>
     </row>
-    <row r="6" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="8" t="s">
+    <row r="20" spans="1:10" s="7" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="V6" s="9"/>
-      <c r="W6" s="9"/>
-      <c r="X6" s="9"/>
-      <c r="Y6" s="9"/>
-      <c r="Z6" s="9"/>
-      <c r="AA6" s="9"/>
-      <c r="AB6" s="9"/>
-      <c r="AC6" s="9"/>
-      <c r="AD6" s="9"/>
-      <c r="AE6" s="9"/>
-      <c r="AF6" s="9"/>
-      <c r="AG6" s="9"/>
-      <c r="AH6" s="9"/>
-      <c r="AI6" s="9"/>
-      <c r="AJ6" s="9"/>
-      <c r="AK6" s="9"/>
-      <c r="AL6" s="9"/>
-      <c r="AM6" s="9"/>
     </row>
-    <row r="7" spans="1:39" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
-      <c r="U7" s="9"/>
-      <c r="V7" s="9"/>
-      <c r="W7" s="9"/>
-      <c r="X7" s="9"/>
-      <c r="Y7" s="9"/>
-      <c r="Z7" s="9"/>
-      <c r="AA7" s="9"/>
-      <c r="AB7" s="9"/>
-      <c r="AC7" s="9"/>
-      <c r="AD7" s="9"/>
-      <c r="AE7" s="9"/>
-      <c r="AF7" s="9"/>
-      <c r="AG7" s="9"/>
-      <c r="AH7" s="9"/>
-      <c r="AI7" s="9"/>
-      <c r="AJ7" s="9"/>
-      <c r="AK7" s="9"/>
-      <c r="AL7" s="9"/>
-      <c r="AM7" s="9"/>
-    </row>
-    <row r="8" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="9"/>
-      <c r="S8" s="9"/>
-      <c r="T8" s="9"/>
-      <c r="U8" s="9"/>
-      <c r="V8" s="9"/>
-      <c r="W8" s="9"/>
-      <c r="X8" s="9"/>
-      <c r="Y8" s="9"/>
-      <c r="Z8" s="9"/>
-      <c r="AA8" s="9"/>
-      <c r="AB8" s="9"/>
-      <c r="AC8" s="9"/>
-      <c r="AD8" s="9"/>
-      <c r="AE8" s="9"/>
-      <c r="AF8" s="9"/>
-      <c r="AG8" s="9"/>
-      <c r="AH8" s="9"/>
-      <c r="AI8" s="9"/>
-      <c r="AJ8" s="9"/>
-      <c r="AK8" s="9"/>
-      <c r="AL8" s="9"/>
-      <c r="AM8" s="9"/>
-    </row>
-    <row r="9" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D9" s="10"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="15"/>
-      <c r="S9" s="12"/>
-    </row>
-    <row r="10" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="15"/>
-      <c r="S10" s="15"/>
-      <c r="T10" s="15"/>
-      <c r="U10" s="15"/>
-      <c r="V10" s="15"/>
-      <c r="W10" s="15"/>
-      <c r="X10" s="15"/>
-      <c r="Y10" s="15"/>
-      <c r="Z10" s="15"/>
-      <c r="AA10" s="15"/>
-      <c r="AB10" s="15"/>
-      <c r="AC10" s="15"/>
-      <c r="AD10" s="15"/>
-      <c r="AE10" s="15"/>
-      <c r="AF10" s="15"/>
-      <c r="AG10" s="15"/>
-      <c r="AH10" s="15"/>
-      <c r="AI10" s="15"/>
-      <c r="AJ10" s="15"/>
-      <c r="AK10" s="15"/>
-      <c r="AL10" s="15"/>
-      <c r="AM10" s="15"/>
-    </row>
-    <row r="11" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
-      <c r="T11" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="U11" s="15"/>
-      <c r="V11" s="15"/>
-      <c r="W11" s="15"/>
-      <c r="X11" s="15"/>
-      <c r="Y11" s="15"/>
-      <c r="Z11" s="15"/>
-      <c r="AA11" s="15"/>
-      <c r="AB11" s="15"/>
-      <c r="AC11" s="15"/>
-      <c r="AD11" s="15"/>
-      <c r="AE11" s="15"/>
-      <c r="AF11" s="15"/>
-      <c r="AG11" s="15"/>
-      <c r="AH11" s="15"/>
-      <c r="AI11" s="15"/>
-      <c r="AJ11" s="15"/>
-      <c r="AK11" s="15"/>
-      <c r="AL11" s="15"/>
-      <c r="AM11" s="15"/>
-    </row>
-    <row r="12" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="15"/>
-      <c r="S12" s="15"/>
-      <c r="T12" s="15"/>
-      <c r="U12" s="15"/>
-      <c r="V12" s="15"/>
-      <c r="W12" s="15"/>
-      <c r="X12" s="15"/>
-      <c r="Y12" s="15"/>
-      <c r="Z12" s="15"/>
-      <c r="AA12" s="15"/>
-      <c r="AB12" s="15"/>
-      <c r="AC12" s="15"/>
-      <c r="AD12" s="15"/>
-      <c r="AE12" s="15"/>
-      <c r="AF12" s="15"/>
-      <c r="AG12" s="15"/>
-      <c r="AH12" s="15"/>
-      <c r="AI12" s="15"/>
-      <c r="AJ12" s="15"/>
-      <c r="AK12" s="15"/>
-      <c r="AL12" s="15"/>
-      <c r="AM12" s="15"/>
-    </row>
-    <row r="13" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="J13" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="15"/>
-      <c r="S13" s="15"/>
-      <c r="T13" s="15"/>
-      <c r="U13" s="15"/>
-      <c r="V13" s="15"/>
-      <c r="W13" s="15"/>
-      <c r="X13" s="15"/>
-      <c r="Y13" s="15"/>
-      <c r="Z13" s="15"/>
-      <c r="AA13" s="15"/>
-      <c r="AB13" s="15"/>
-      <c r="AC13" s="15"/>
-      <c r="AD13" s="15"/>
-      <c r="AE13" s="15"/>
-      <c r="AF13" s="15"/>
-      <c r="AG13" s="15"/>
-      <c r="AH13" s="15"/>
-      <c r="AI13" s="15"/>
-      <c r="AJ13" s="15"/>
-      <c r="AK13" s="15"/>
-      <c r="AL13" s="15"/>
-      <c r="AM13" s="15"/>
-    </row>
-    <row r="14" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="15"/>
-      <c r="S14" s="15"/>
-      <c r="T14" s="15"/>
-      <c r="U14" s="15"/>
-      <c r="V14" s="15"/>
-      <c r="W14" s="15"/>
-      <c r="X14" s="15"/>
-      <c r="Y14" s="15"/>
-      <c r="Z14" s="15"/>
-      <c r="AA14" s="15"/>
-      <c r="AB14" s="15"/>
-      <c r="AC14" s="15"/>
-      <c r="AD14" s="15"/>
-      <c r="AE14" s="15"/>
-      <c r="AF14" s="15"/>
-      <c r="AG14" s="15"/>
-      <c r="AH14" s="15"/>
-      <c r="AI14" s="15"/>
-      <c r="AJ14" s="15"/>
-      <c r="AK14" s="15"/>
-      <c r="AL14" s="15"/>
-      <c r="AM14" s="15"/>
-    </row>
-    <row r="15" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="G15" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="15"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="15"/>
-      <c r="S15" s="15"/>
-      <c r="T15" s="15"/>
-      <c r="U15" s="15"/>
-      <c r="V15" s="15"/>
-      <c r="W15" s="15"/>
-      <c r="X15" s="15"/>
-      <c r="Y15" s="15"/>
-      <c r="Z15" s="15"/>
-      <c r="AA15" s="15"/>
-      <c r="AB15" s="15"/>
-      <c r="AC15" s="15"/>
-      <c r="AD15" s="15"/>
-      <c r="AE15" s="15"/>
-      <c r="AF15" s="15"/>
-      <c r="AG15" s="15"/>
-      <c r="AH15" s="15"/>
-      <c r="AI15" s="15"/>
-      <c r="AJ15" s="15"/>
-      <c r="AK15" s="15"/>
-      <c r="AL15" s="15"/>
-      <c r="AM15" s="15"/>
-    </row>
-    <row r="16" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="G16" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="15"/>
-      <c r="S16" s="15"/>
-      <c r="T16" s="15"/>
-      <c r="U16" s="15"/>
-      <c r="V16" s="15"/>
-      <c r="W16" s="15"/>
-      <c r="X16" s="15"/>
-      <c r="Y16" s="15"/>
-      <c r="Z16" s="15"/>
-      <c r="AA16" s="15"/>
-      <c r="AB16" s="15"/>
-      <c r="AC16" s="15"/>
-      <c r="AD16" s="15"/>
-      <c r="AE16" s="15"/>
-      <c r="AF16" s="15"/>
-      <c r="AG16" s="15"/>
-      <c r="AH16" s="15"/>
-      <c r="AI16" s="15"/>
-      <c r="AJ16" s="15"/>
-      <c r="AK16" s="15"/>
-      <c r="AL16" s="15"/>
-      <c r="AM16" s="15"/>
-    </row>
-    <row r="17" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="15"/>
-      <c r="S17" s="15"/>
-      <c r="T17" s="15"/>
-      <c r="U17" s="15"/>
-      <c r="V17" s="15"/>
-      <c r="W17" s="15"/>
-      <c r="X17" s="15"/>
-      <c r="Y17" s="15"/>
-      <c r="Z17" s="15"/>
-      <c r="AA17" s="15"/>
-      <c r="AB17" s="15"/>
-      <c r="AC17" s="15"/>
-      <c r="AD17" s="15"/>
-      <c r="AE17" s="15"/>
-      <c r="AF17" s="15"/>
-      <c r="AG17" s="15"/>
-      <c r="AH17" s="15"/>
-      <c r="AI17" s="15"/>
-      <c r="AJ17" s="15"/>
-      <c r="AK17" s="15"/>
-      <c r="AL17" s="15"/>
-      <c r="AM17" s="15"/>
-    </row>
-    <row r="18" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="15"/>
-      <c r="P18" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q18" s="15"/>
-      <c r="R18" s="15"/>
-      <c r="S18" s="15"/>
-      <c r="T18" s="15"/>
-      <c r="U18" s="15"/>
-      <c r="V18" s="15"/>
-      <c r="W18" s="15"/>
-      <c r="X18" s="15"/>
-      <c r="Y18" s="15"/>
-      <c r="Z18" s="15"/>
-      <c r="AA18" s="15"/>
-      <c r="AB18" s="15"/>
-      <c r="AC18" s="15"/>
-      <c r="AD18" s="15"/>
-      <c r="AE18" s="15"/>
-      <c r="AF18" s="15"/>
-      <c r="AG18" s="15"/>
-      <c r="AH18" s="15"/>
-      <c r="AI18" s="15"/>
-      <c r="AJ18" s="15"/>
-      <c r="AK18" s="15"/>
-      <c r="AL18" s="15"/>
-      <c r="AM18" s="15"/>
-    </row>
-    <row r="19" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="15"/>
-      <c r="O19" s="15"/>
-      <c r="P19" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q19" s="15"/>
-      <c r="R19" s="15"/>
-      <c r="S19" s="15"/>
-      <c r="T19" s="15"/>
-      <c r="U19" s="15"/>
-      <c r="V19" s="15"/>
-      <c r="W19" s="15"/>
-      <c r="X19" s="15"/>
-      <c r="Y19" s="15"/>
-      <c r="Z19" s="15"/>
-      <c r="AA19" s="15"/>
-      <c r="AB19" s="15"/>
-      <c r="AC19" s="15"/>
-      <c r="AD19" s="15"/>
-      <c r="AE19" s="15"/>
-      <c r="AF19" s="15"/>
-      <c r="AG19" s="15"/>
-      <c r="AH19" s="15"/>
-      <c r="AI19" s="15"/>
-      <c r="AJ19" s="15"/>
-      <c r="AK19" s="15"/>
-      <c r="AL19" s="15"/>
-      <c r="AM19" s="15"/>
-    </row>
-    <row r="20" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="15"/>
-      <c r="R20" s="15"/>
-      <c r="S20" s="15"/>
-      <c r="T20" s="15"/>
-      <c r="U20" s="15"/>
-      <c r="V20" s="15"/>
-      <c r="W20" s="15"/>
-      <c r="X20" s="15"/>
-      <c r="Y20" s="15"/>
-      <c r="Z20" s="15"/>
-      <c r="AA20" s="15"/>
-      <c r="AB20" s="15"/>
-      <c r="AC20" s="15"/>
-      <c r="AD20" s="15"/>
-      <c r="AE20" s="15"/>
-      <c r="AF20" s="15"/>
-      <c r="AG20" s="15"/>
-      <c r="AH20" s="15"/>
-      <c r="AI20" s="15"/>
-      <c r="AJ20" s="15"/>
-      <c r="AK20" s="15"/>
-      <c r="AL20" s="15"/>
-      <c r="AM20" s="15"/>
-    </row>
-    <row r="21" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="15"/>
-      <c r="S21" s="15"/>
-      <c r="T21" s="15"/>
-      <c r="U21" s="15"/>
-      <c r="V21" s="15"/>
-      <c r="W21" s="15"/>
-      <c r="X21" s="15"/>
-      <c r="Y21" s="15"/>
-      <c r="Z21" s="15"/>
-      <c r="AA21" s="15"/>
-      <c r="AB21" s="15"/>
-      <c r="AC21" s="15"/>
-      <c r="AD21" s="15"/>
-      <c r="AE21" s="15"/>
-      <c r="AF21" s="15"/>
-      <c r="AG21" s="15"/>
-      <c r="AH21" s="15"/>
-      <c r="AI21" s="15"/>
-      <c r="AJ21" s="15"/>
-      <c r="AK21" s="15"/>
-      <c r="AL21" s="15"/>
-      <c r="AM21" s="15"/>
-    </row>
-    <row r="22" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="23" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="26" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="30" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="31" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="32" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2679,7 +1703,6 @@
     <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="landscape"/>
@@ -2705,45 +1728,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="20" t="s">
+      <c r="A1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>5</v>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>61</v>
+      <c r="A2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="22" t="s">
-        <v>63</v>
+      <c r="A3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3750,38 +2773,38 @@
   <sheetData>
     <row r="1" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C2" s="23" t="str">
+        <v>55</v>
+      </c>
+      <c r="C2" s="6" t="str">
         <f ca="1">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2023-10-20 6-56</v>
+        <v>2023-11-22 11-58</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>